<commit_message>
Almost Sent Done :weary: / New TamirRequset API manual updated :wink:
</commit_message>
<xml_diff>
--- a/WebServices (Without SP)/1400/03_خرداد/راهنمای وب سرویس_ ثبت درخواست اولیه خاموشی بابرنامه14000319.xlsx
+++ b/WebServices (Without SP)/1400/03_خرداد/راهنمای وب سرویس_ ثبت درخواست اولیه خاموشی بابرنامه14000319.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\WebServices (Without SP)\1400\خرداد\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\WebServices (Without SP)\1400\03_خرداد\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A722E937-4348-4D3E-829F-A8D10714120B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3978FD-F2C7-4A42-8F8E-A683D131D765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -277,6 +277,36 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">
+{
+    "Message": "TamirRequest Successfully Inserted/Updated...",
+    "IsSuccessfull": true,
+    "Data": 9900000000000033
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">راهنمای وب سرویس‌ ثبت درخواست اولیه خاموشی بابرنامه
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Mitra"/>
+        <charset val="178"/>
+      </rPr>
+      <t>تذرو افزار 14000319</t>
+    </r>
+  </si>
+  <si>
+    <t>http://IPAddress/NewTamirRequest</t>
+  </si>
+  <si>
+    <t>نام وب متد:  Maz_SetRequestTamir</t>
+  </si>
+  <si>
     <t>{
  "TamirId" : 9900000000000033,
  "TamirInfo" : {
@@ -292,7 +322,7 @@
         "WorkingAddress": "Run your own business !!!",
         "GpsX": 121654.5416,
         "GpsY": 123456.222,
-        "CriticalsAddress": "Don't be nosy",
+        "CriticalsAddress": "شهرری خیابان امام",
         "IsInCityService": 0,
         "NetworkType": "MP",
         "OperationList": [
@@ -318,36 +348,6 @@
          ]
  }
 }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-{
-    "Message": "TamirRequest Successfully Inserted/Updated...",
-    "IsSuccessfull": true,
-    "Data": 9900000000000033
-}</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">راهنمای وب سرویس‌ ثبت درخواست اولیه خاموشی بابرنامه
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="B Mitra"/>
-        <charset val="178"/>
-      </rPr>
-      <t>تذرو افزار 14000319</t>
-    </r>
-  </si>
-  <si>
-    <t>http://IPAddress/NewTamirRequest</t>
-  </si>
-  <si>
-    <t>نام وب متد:  Maz_SetRequestTamir</t>
   </si>
 </sst>
 </file>
@@ -1344,8 +1344,8 @@
   </sheetPr>
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35:D35"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,7 +1357,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
@@ -1373,7 +1373,7 @@
     </row>
     <row r="3" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>6</v>
@@ -1391,7 +1391,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4" s="47"/>
     </row>
@@ -1837,11 +1837,11 @@
     </row>
     <row r="38" spans="1:4" ht="399.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B38" s="35"/>
       <c r="C38" s="36" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D38" s="37"/>
     </row>

</xml_diff>